<commit_message>
gen() now outputs correct recensoring variable (internal calculation was already correct) test now defaults to cox if adjvars is specified (but not ipe) updated my details in help file
</commit_message>
<xml_diff>
--- a/strbee-to-do.xlsx
+++ b/strbee-to-do.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>DONE</t>
   </si>
@@ -88,13 +88,31 @@
   </si>
   <si>
     <t>Irene Santi</t>
+  </si>
+  <si>
+    <t>recensoring seems to have no effect</t>
+  </si>
+  <si>
+    <t>UMIT course participants</t>
+  </si>
+  <si>
+    <t>should gen() work with simple psi()?</t>
+  </si>
+  <si>
+    <t>Adj(x) should imply test(cox)</t>
+  </si>
+  <si>
+    <t>made this the default</t>
+  </si>
+  <si>
+    <t>this was correct behaviour specific to that problem - wrote notes in UMIT folder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +144,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -203,12 +227,65 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="8"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -549,13 +626,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,116 +767,142 @@
         <v>43117</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5">
+        <v>43209</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <v>43250</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5">
-        <v>42373</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
+        <v>43209</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43250</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5">
+        <v>42373</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="4"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="9"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="4"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="9"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="4"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="9"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="4"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="9"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="4"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="9"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="4"/>
       <c r="E23" s="7"/>
     </row>
@@ -824,52 +927,112 @@
       <c r="D26" s="4"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="9"/>
       <c r="D27" s="4"/>
       <c r="E27" s="7"/>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A15:A17 A13 A4:A9">
-    <cfRule type="expression" dxfId="7" priority="13">
+  <conditionalFormatting sqref="A21:A22 A18 A4:A8 A14">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>ISBLANK($E4)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="13" priority="12">
+      <formula>ISBLANK($E17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="expression" dxfId="12" priority="11">
+      <formula>ISBLANK($E16)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="expression" dxfId="11" priority="10">
+      <formula>ISBLANK($E23)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="expression" dxfId="10" priority="9">
+      <formula>ISBLANK($E24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A32">
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>ISBLANK($E25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="expression" dxfId="8" priority="6">
+      <formula>ISBLANK($E19)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="expression" dxfId="7" priority="21">
+      <formula>ISBLANK(#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>ISBLANK($E9)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>ISBLANK($E10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>ISBLANK($E13)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>ISBLANK($E12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>ISBLANK($E11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>ISBLANK($E18)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ISBLANK($E19)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A27">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>ISBLANK($E20)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISBLANK($E14)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="0" priority="16">
-      <formula>ISBLANK(#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>